<commit_message>
Bug fix for actual/start price
</commit_message>
<xml_diff>
--- a/Trades.xlsx
+++ b/Trades.xlsx
@@ -2226,7 +2226,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>589 950,00 ₽</t>
+          <t>621 000,00 ₽</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -5848,7 +5848,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>189 000,00 ₽</t>
+          <t>216 000,00 ₽</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
@@ -5885,7 +5885,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>3 600 000,00 ₽</t>
+          <t>4 500 000,00 ₽</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
@@ -5922,7 +5922,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>523 530,00 ₽</t>
+          <t>747 900,00 ₽</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -5969,7 +5969,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>269 640,00 ₽</t>
+          <t>385 200,00 ₽</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -6680,7 +6680,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>1 782 135,00 ₽</t>
+          <t>2 072 250,00 ₽</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
@@ -6990,7 +6990,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>185 130,00 ₽</t>
+          <t>217 800,00 ₽</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
@@ -7037,7 +7037,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>229 500,00 ₽</t>
+          <t>270 000,00 ₽</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
@@ -7084,7 +7084,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>31 500,00 ₽</t>
+          <t>63 000,00 ₽</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
@@ -7131,7 +7131,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>47 250,00 ₽</t>
+          <t>94 500,00 ₽</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
@@ -8035,7 +8035,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>78 710,40 ₽</t>
+          <t>131 184,00 ₽</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
@@ -8082,7 +8082,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>27 000,00 ₽</t>
+          <t>45 000,00 ₽</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
@@ -8129,7 +8129,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>158 035 890,00 ₽</t>
+          <t>166 353 568,43 ₽</t>
         </is>
       </c>
       <c r="G181" t="inlineStr">
@@ -8166,7 +8166,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>37 800,00 ₽</t>
+          <t>63 000,00 ₽</t>
         </is>
       </c>
       <c r="G182" t="inlineStr">
@@ -8203,7 +8203,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>57 240,00 ₽</t>
+          <t>95 400,00 ₽</t>
         </is>
       </c>
       <c r="G183" t="inlineStr">
@@ -8240,7 +8240,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>192 069,90 ₽</t>
+          <t>213 411,00 ₽</t>
         </is>
       </c>
       <c r="G184" t="inlineStr">
@@ -8277,7 +8277,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>46 838,40 ₽</t>
+          <t>54 630,00 ₽</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
@@ -8325,7 +8325,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>49 973,76 ₽</t>
+          <t>116 091,90 ₽</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
@@ -8372,7 +8372,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>1 074 287,61 ₽</t>
+          <t>1 342 859,49 ₽</t>
         </is>
       </c>
       <c r="G187" t="inlineStr">
@@ -8409,7 +8409,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>308 448,00 ₽</t>
+          <t>385 560,00 ₽</t>
         </is>
       </c>
       <c r="G188" t="inlineStr">
@@ -8446,7 +8446,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>2 525 040,00 ₽</t>
+          <t>3 607 200,00 ₽</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
@@ -8491,7 +8491,7 @@
   <dimension ref="A1:I189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10366,7 +10366,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>589 950,00 ₽</t>
+          <t>621 000,00 ₽</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -13989,7 +13989,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>189 000,00 ₽</t>
+          <t>216 000,00 ₽</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
@@ -14026,7 +14026,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>3 600 000,00 ₽</t>
+          <t>4 500 000,00 ₽</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
@@ -14063,7 +14063,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>523 530,00 ₽</t>
+          <t>747 900,00 ₽</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -14110,7 +14110,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>269 640,00 ₽</t>
+          <t>385 200,00 ₽</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -14821,7 +14821,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>1 782 135,00 ₽</t>
+          <t>2 072 250,00 ₽</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
@@ -15131,7 +15131,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>185 130,00 ₽</t>
+          <t>217 800,00 ₽</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
@@ -15178,7 +15178,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>229 500,00 ₽</t>
+          <t>270 000,00 ₽</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
@@ -15225,7 +15225,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>31 500,00 ₽</t>
+          <t>63 000,00 ₽</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
@@ -15272,7 +15272,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>47 250,00 ₽</t>
+          <t>94 500,00 ₽</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
@@ -16176,7 +16176,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>78 710,40 ₽</t>
+          <t>131 184,00 ₽</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
@@ -16223,7 +16223,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>27 000,00 ₽</t>
+          <t>45 000,00 ₽</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
@@ -16270,7 +16270,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>158 035 890,00 ₽</t>
+          <t>166 353 568,43 ₽</t>
         </is>
       </c>
       <c r="G181" t="inlineStr">
@@ -16307,7 +16307,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>37 800,00 ₽</t>
+          <t>63 000,00 ₽</t>
         </is>
       </c>
       <c r="G182" t="inlineStr">
@@ -16344,7 +16344,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>57 240,00 ₽</t>
+          <t>95 400,00 ₽</t>
         </is>
       </c>
       <c r="G183" t="inlineStr">
@@ -16381,7 +16381,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>192 069,90 ₽</t>
+          <t>213 411,00 ₽</t>
         </is>
       </c>
       <c r="G184" t="inlineStr">
@@ -16418,7 +16418,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>46 838,40 ₽</t>
+          <t>54 630,00 ₽</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
@@ -16466,7 +16466,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>49 973,76 ₽</t>
+          <t>116 091,90 ₽</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
@@ -16513,7 +16513,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>1 074 287,61 ₽</t>
+          <t>1 342 859,49 ₽</t>
         </is>
       </c>
       <c r="G187" t="inlineStr">
@@ -16550,7 +16550,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>308 448,00 ₽</t>
+          <t>385 560,00 ₽</t>
         </is>
       </c>
       <c r="G188" t="inlineStr">
@@ -16587,7 +16587,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>2 525 040,00 ₽</t>
+          <t>3 607 200,00 ₽</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">

</xml_diff>